<commit_message>
In README tutorial, added comment for calculateFingerprint. In genotypeMap templates, added instructions to not start group name with a digit.
</commit_message>
<xml_diff>
--- a/genotypeMap_templates/YYMMDD_BX_genotypeMap.xlsx
+++ b/genotypeMap_templates/YYMMDD_BX_genotypeMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francoiskroll/Dropbox/phd/utilities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francoiskroll/Dropbox/FramebyFrame/genotypeMap_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3B54EC-21F6-D24D-B584-B33A00220481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4302E1-D53F-FC44-822B-D8A8978CFABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{ED68630C-B3B4-954B-A30D-3426C59A8FBE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{ED68630C-B3B4-954B-A30D-3426C59A8FBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="43">
   <si>
     <t>H</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>other tips</t>
+  </si>
+  <si>
+    <t>– Do not start a group name with a number. For example, use WT1 instead of 1WT.</t>
   </si>
 </sst>
 </file>
@@ -501,7 +504,7 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -520,7 +523,6 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="9"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="10"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="11"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="empty" xfId="3" xr:uid="{B5FCBFC7-15E7-B149-8620-A603EEE586BD}"/>
@@ -855,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{437C1C92-2EB9-1F4F-88EA-AA3B05441A17}">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1263,17 +1265,17 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="18" t="s">
+      <c r="B21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="A23" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1350,6 +1352,11 @@
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>